<commit_message>
Atualização na planilha das sprints
</commit_message>
<xml_diff>
--- a/Código de cores/tabela alerta cores.xlsx
+++ b/Código de cores/tabela alerta cores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Faculdade Breno\PROJETO PI\Sixsolution-project\Código de cores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Faculdade Breno\sixsolution\Sixsolution-project\Código de cores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A08F87-CAA8-4935-8A82-903D7C0C46F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EDB4F6-EE3F-4EB7-885C-7D2AA654B83D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -497,6 +497,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -513,9 +516,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -15143,7 +15143,7 @@
   <dimension ref="C3:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15374,14 +15374,14 @@
       <c r="N18" s="2"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
       <c r="I19" s="1"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -15555,7 +15555,7 @@
       <c r="E26" s="26">
         <v>23</v>
       </c>
-      <c r="F26" s="37" t="s">
+      <c r="F26" s="31" t="s">
         <v>33</v>
       </c>
       <c r="G26" s="27">
@@ -15581,13 +15581,13 @@
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C28" s="11"/>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="34"/>
       <c r="I28" s="1"/>
       <c r="J28" s="2"/>
       <c r="K28" s="3"/>
@@ -15627,7 +15627,7 @@
       <c r="E30" s="15">
         <v>0.65</v>
       </c>
-      <c r="F30" s="37" t="s">
+      <c r="F30" s="31" t="s">
         <v>42</v>
       </c>
       <c r="G30" s="16">

</xml_diff>